<commit_message>
added more combos and identified unsupported
</commit_message>
<xml_diff>
--- a/calc_rules.xlsx
+++ b/calc_rules.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\msys64\home\Joh\OasisLMF_branch\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{AE6DAF0B-32C3-4FFF-B2C1-37F3D60D9F04}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD7143A0-733F-4F6C-851D-9805BADEEA13}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="193" uniqueCount="161">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="165">
   <si>
     <t>desc</t>
   </si>
@@ -516,6 +516,18 @@
   </si>
   <si>
     <t>no deductible % loss with min and max deductible and limit % TIV</t>
+  </si>
+  <si>
+    <t>deductible % loss with min deductible and limit</t>
+  </si>
+  <si>
+    <t>deductible % loss with max deductible and limit</t>
+  </si>
+  <si>
+    <t>deductible % loss with min deductible and limit % TIV</t>
+  </si>
+  <si>
+    <t>deductible % loss with max deductible and limit % TIV</t>
   </si>
 </sst>
 </file>
@@ -1356,13 +1368,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:O147"/>
+  <dimension ref="A1:O151"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B118" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="O1" sqref="O1"/>
+      <selection pane="bottomRight" activeCell="A148" sqref="A148:M151"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1476,7 +1488,7 @@
         <v>(1, 0, 0, 1, 0, 0, 0, 0, 0, 0)</v>
       </c>
       <c r="O2">
-        <f>COUNTIF($M$2:$M$147,M2)</f>
+        <f t="shared" ref="O2:O33" si="1">COUNTIF($M$2:$M$147,M2)</f>
         <v>1</v>
       </c>
     </row>
@@ -1522,7 +1534,7 @@
         <v>(1, 0, 0, 1, 0, 0, 2, 0, 0, 0)</v>
       </c>
       <c r="O3">
-        <f>COUNTIF($M$2:$M$147,M3)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
@@ -1568,7 +1580,7 @@
         <v>(0, 0, 0, 1, 1, 0, 0, 0, 0, 0)</v>
       </c>
       <c r="O4">
-        <f>COUNTIF($M$2:$M$147,M4)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
@@ -1614,7 +1626,7 @@
         <v>(0, 0, 0, 1, 1, 0, 2, 0, 0, 0)</v>
       </c>
       <c r="O5">
-        <f>COUNTIF($M$2:$M$147,M5)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
@@ -1660,7 +1672,7 @@
         <v>(0, 0, 0, 1, 1, 1, 0, 0, 0, 0)</v>
       </c>
       <c r="O6">
-        <f>COUNTIF($M$2:$M$147,M6)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
@@ -1706,7 +1718,7 @@
         <v>(0, 0, 0, 1, 1, 1, 2, 0, 0, 0)</v>
       </c>
       <c r="O7">
-        <f>COUNTIF($M$2:$M$147,M7)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
@@ -1752,7 +1764,7 @@
         <v>(1, 0, 0, 1, 1, 0, 2, 0, 0, 0)</v>
       </c>
       <c r="O8">
-        <f>COUNTIF($M$2:$M$147,M8)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
@@ -1798,7 +1810,7 @@
         <v>(1, 0, 0, 1, 1, 0, 0, 0, 0, 0)</v>
       </c>
       <c r="O9">
-        <f>COUNTIF($M$2:$M$147,M9)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
@@ -1844,7 +1856,7 @@
         <v>(1, 0, 0, 1, 1, 1, 2, 0, 0, 0)</v>
       </c>
       <c r="O10">
-        <f>COUNTIF($M$2:$M$147,M10)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
@@ -1890,7 +1902,7 @@
         <v>(1, 0, 0, 1, 1, 1, 0, 0, 0, 0)</v>
       </c>
       <c r="O11">
-        <f>COUNTIF($M$2:$M$147,M11)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
@@ -1936,7 +1948,7 @@
         <v>(1, 0, 0, 1, 0, 0, 0, 2, 0, 0)</v>
       </c>
       <c r="O12">
-        <f>COUNTIF($M$2:$M$147,M12)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
@@ -1978,11 +1990,11 @@
         <v>0</v>
       </c>
       <c r="M13" t="str">
-        <f t="shared" ref="M13:M14" si="1">"("&amp;C13&amp;", "&amp;D13&amp;", "&amp;E13&amp;", "&amp;F13&amp;", "&amp;G13&amp;", "&amp;H13&amp;", "&amp;I13&amp;", "&amp;J13&amp;", "&amp;K13&amp;", "&amp;L13&amp;")"</f>
+        <f t="shared" ref="M13:M14" si="2">"("&amp;C13&amp;", "&amp;D13&amp;", "&amp;E13&amp;", "&amp;F13&amp;", "&amp;G13&amp;", "&amp;H13&amp;", "&amp;I13&amp;", "&amp;J13&amp;", "&amp;K13&amp;", "&amp;L13&amp;")"</f>
         <v>(1, 0, 0, 1, 0, 0, 2, 2, 0, 0)</v>
       </c>
       <c r="O13">
-        <f>COUNTIF($M$2:$M$147,M13)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
@@ -2024,11 +2036,11 @@
         <v>0</v>
       </c>
       <c r="M14" t="str">
+        <f t="shared" si="2"/>
+        <v>(1, 0, 0, 1, 0, 0, 0, 2, 2, 0)</v>
+      </c>
+      <c r="O14">
         <f t="shared" si="1"/>
-        <v>(1, 0, 0, 1, 0, 0, 0, 2, 2, 0)</v>
-      </c>
-      <c r="O14">
-        <f>COUNTIF($M$2:$M$147,M14)</f>
         <v>1</v>
       </c>
     </row>
@@ -2074,7 +2086,7 @@
         <v>(1, 0, 0, 1, 0, 0, 1, 0, 1, 0)</v>
       </c>
       <c r="O15">
-        <f>COUNTIF($M$2:$M$147,M15)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
@@ -2120,7 +2132,7 @@
         <v>(0, 0, 1, 1, 0, 0, 0, 0, 0, 0)</v>
       </c>
       <c r="O16">
-        <f>COUNTIF($M$2:$M$147,M16)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
@@ -2166,7 +2178,7 @@
         <v>(0, 0, 1, 1, 0, 0, 1, 0, 0, 0)</v>
       </c>
       <c r="O17">
-        <f>COUNTIF($M$2:$M$147,M17)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
@@ -2212,7 +2224,7 @@
         <v>(0, 0, 1, 1, 0, 0, 2, 0, 0, 0)</v>
       </c>
       <c r="O18">
-        <f>COUNTIF($M$2:$M$147,M18)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
@@ -2254,11 +2266,11 @@
         <v>0</v>
       </c>
       <c r="M19" t="str">
-        <f t="shared" ref="M19:M23" si="2">"("&amp;C19&amp;", "&amp;D19&amp;", "&amp;E19&amp;", "&amp;F19&amp;", "&amp;G19&amp;", "&amp;H19&amp;", "&amp;I19&amp;", "&amp;J19&amp;", "&amp;K19&amp;", "&amp;L19&amp;")"</f>
+        <f t="shared" ref="M19:M23" si="3">"("&amp;C19&amp;", "&amp;D19&amp;", "&amp;E19&amp;", "&amp;F19&amp;", "&amp;G19&amp;", "&amp;H19&amp;", "&amp;I19&amp;", "&amp;J19&amp;", "&amp;K19&amp;", "&amp;L19&amp;")"</f>
         <v>(0, 0, 1, 1, 0, 0, 0, 0, 2, 0)</v>
       </c>
       <c r="O19">
-        <f>COUNTIF($M$2:$M$147,M19)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
@@ -2300,11 +2312,11 @@
         <v>0</v>
       </c>
       <c r="M20" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>(0, 0, 1, 1, 0, 0, 1, 0, 2, 0)</v>
       </c>
       <c r="O20">
-        <f>COUNTIF($M$2:$M$147,M20)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
@@ -2346,11 +2358,11 @@
         <v>0</v>
       </c>
       <c r="M21" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>(0, 0, 1, 1, 0, 0, 2, 0, 2, 0)</v>
       </c>
       <c r="O21">
-        <f>COUNTIF($M$2:$M$147,M21)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
@@ -2392,14 +2404,14 @@
         <v>0</v>
       </c>
       <c r="M22" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>(1, 0, 1, 1, 0, 0, 0, 0, 0, 0)</v>
       </c>
       <c r="N22" t="s">
         <v>101</v>
       </c>
       <c r="O22">
-        <f>COUNTIF($M$2:$M$147,M22)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
@@ -2441,14 +2453,14 @@
         <v>0</v>
       </c>
       <c r="M23" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>(1, 0, 1, 1, 0, 0, 2, 0, 0, 0)</v>
       </c>
       <c r="N23" t="s">
         <v>101</v>
       </c>
       <c r="O23">
-        <f>COUNTIF($M$2:$M$147,M23)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
@@ -2490,14 +2502,14 @@
         <v>0</v>
       </c>
       <c r="M24" t="str">
-        <f t="shared" ref="M24:M27" si="3">"("&amp;C24&amp;", "&amp;D24&amp;", "&amp;E24&amp;", "&amp;F24&amp;", "&amp;G24&amp;", "&amp;H24&amp;", "&amp;I24&amp;", "&amp;J24&amp;", "&amp;K24&amp;", "&amp;L24&amp;")"</f>
+        <f t="shared" ref="M24:M27" si="4">"("&amp;C24&amp;", "&amp;D24&amp;", "&amp;E24&amp;", "&amp;F24&amp;", "&amp;G24&amp;", "&amp;H24&amp;", "&amp;I24&amp;", "&amp;J24&amp;", "&amp;K24&amp;", "&amp;L24&amp;")"</f>
         <v>(1, 0, 1, 1, 0, 0, 0, 0, 2, 0)</v>
       </c>
       <c r="N24" t="s">
         <v>101</v>
       </c>
       <c r="O24">
-        <f>COUNTIF($M$2:$M$147,M24)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
@@ -2539,14 +2551,14 @@
         <v>0</v>
       </c>
       <c r="M25" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>(1, 0, 1, 1, 0, 0, 2, 0, 2, 0)</v>
       </c>
       <c r="N25" t="s">
         <v>101</v>
       </c>
       <c r="O25">
-        <f>COUNTIF($M$2:$M$147,M25)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
@@ -2588,14 +2600,14 @@
         <v>0</v>
       </c>
       <c r="M26" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>(1, 1, 1, 1, 0, 0, 0, 0, 0, 0)</v>
       </c>
       <c r="N26" t="s">
         <v>101</v>
       </c>
       <c r="O26">
-        <f>COUNTIF($M$2:$M$147,M26)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
@@ -2637,14 +2649,14 @@
         <v>0</v>
       </c>
       <c r="M27" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>(1, 1, 1, 1, 0, 0, 2, 0, 0, 0)</v>
       </c>
       <c r="N27" t="s">
         <v>101</v>
       </c>
       <c r="O27">
-        <f>COUNTIF($M$2:$M$147,M27)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
@@ -2686,14 +2698,14 @@
         <v>0</v>
       </c>
       <c r="M28" t="str">
-        <f t="shared" ref="M28:M33" si="4">"("&amp;C28&amp;", "&amp;D28&amp;", "&amp;E28&amp;", "&amp;F28&amp;", "&amp;G28&amp;", "&amp;H28&amp;", "&amp;I28&amp;", "&amp;J28&amp;", "&amp;K28&amp;", "&amp;L28&amp;")"</f>
+        <f t="shared" ref="M28:M33" si="5">"("&amp;C28&amp;", "&amp;D28&amp;", "&amp;E28&amp;", "&amp;F28&amp;", "&amp;G28&amp;", "&amp;H28&amp;", "&amp;I28&amp;", "&amp;J28&amp;", "&amp;K28&amp;", "&amp;L28&amp;")"</f>
         <v>(1, 1, 1, 1, 0, 0, 0, 0, 2, 0)</v>
       </c>
       <c r="N28" t="s">
         <v>101</v>
       </c>
       <c r="O28">
-        <f>COUNTIF($M$2:$M$147,M28)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
@@ -2735,14 +2747,14 @@
         <v>0</v>
       </c>
       <c r="M29" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>(1, 1, 1, 1, 0, 0, 2, 0, 2, 0)</v>
       </c>
       <c r="N29" t="s">
         <v>101</v>
       </c>
       <c r="O29">
-        <f>COUNTIF($M$2:$M$147,M29)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
@@ -2784,14 +2796,14 @@
         <v>0</v>
       </c>
       <c r="M30" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>(0, 1, 1, 1, 0, 0, 0, 0, 0, 0)</v>
       </c>
       <c r="N30" t="s">
         <v>101</v>
       </c>
       <c r="O30">
-        <f>COUNTIF($M$2:$M$147,M30)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
@@ -2833,14 +2845,14 @@
         <v>0</v>
       </c>
       <c r="M31" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>(0, 1, 1, 1, 0, 0, 2, 0, 0, 0)</v>
       </c>
       <c r="N31" t="s">
         <v>101</v>
       </c>
       <c r="O31">
-        <f>COUNTIF($M$2:$M$147,M31)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
@@ -2882,14 +2894,14 @@
         <v>0</v>
       </c>
       <c r="M32" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>(0, 1, 1, 1, 0, 0, 0, 0, 2, 0)</v>
       </c>
       <c r="N32" t="s">
         <v>101</v>
       </c>
       <c r="O32">
-        <f>COUNTIF($M$2:$M$147,M32)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
@@ -2931,14 +2943,14 @@
         <v>0</v>
       </c>
       <c r="M33" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>(0, 1, 1, 1, 0, 0, 2, 0, 2, 0)</v>
       </c>
       <c r="N33" t="s">
         <v>101</v>
       </c>
       <c r="O33">
-        <f>COUNTIF($M$2:$M$147,M33)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
@@ -2984,7 +2996,7 @@
         <v>(0, 1, 0, 1, 0, 0, 0, 0, 0, 0)</v>
       </c>
       <c r="O34">
-        <f>COUNTIF($M$2:$M$147,M34)</f>
+        <f t="shared" ref="O34:O65" si="6">COUNTIF($M$2:$M$147,M34)</f>
         <v>1</v>
       </c>
     </row>
@@ -3030,7 +3042,7 @@
         <v>(0, 1, 0, 1, 0, 0, 1, 0, 0, 0)</v>
       </c>
       <c r="O35">
-        <f>COUNTIF($M$2:$M$147,M35)</f>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
     </row>
@@ -3076,7 +3088,7 @@
         <v>(0, 1, 0, 1, 0, 0, 2, 0, 0, 0)</v>
       </c>
       <c r="O36">
-        <f>COUNTIF($M$2:$M$147,M36)</f>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
     </row>
@@ -3122,7 +3134,7 @@
         <v>(0, 1, 0, 1, 0, 0, 0, 0, 2, 0)</v>
       </c>
       <c r="O37">
-        <f>COUNTIF($M$2:$M$147,M37)</f>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
     </row>
@@ -3168,7 +3180,7 @@
         <v>(0, 1, 0, 1, 0, 0, 1, 0, 2, 0)</v>
       </c>
       <c r="O38">
-        <f>COUNTIF($M$2:$M$147,M38)</f>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
     </row>
@@ -3214,7 +3226,7 @@
         <v>(0, 1, 0, 1, 0, 0, 2, 0, 2, 0)</v>
       </c>
       <c r="O39">
-        <f>COUNTIF($M$2:$M$147,M39)</f>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
     </row>
@@ -3256,11 +3268,11 @@
         <v>0</v>
       </c>
       <c r="M40" t="str">
-        <f t="shared" ref="M40:M43" si="5">"("&amp;C40&amp;", "&amp;D40&amp;", "&amp;E40&amp;", "&amp;F40&amp;", "&amp;G40&amp;", "&amp;H40&amp;", "&amp;I40&amp;", "&amp;J40&amp;", "&amp;K40&amp;", "&amp;L40&amp;")"</f>
+        <f t="shared" ref="M40:M43" si="7">"("&amp;C40&amp;", "&amp;D40&amp;", "&amp;E40&amp;", "&amp;F40&amp;", "&amp;G40&amp;", "&amp;H40&amp;", "&amp;I40&amp;", "&amp;J40&amp;", "&amp;K40&amp;", "&amp;L40&amp;")"</f>
         <v>(1, 1, 0, 1, 0, 0, 0, 0, 0, 0)</v>
       </c>
       <c r="O40">
-        <f>COUNTIF($M$2:$M$147,M40)</f>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
     </row>
@@ -3302,11 +3314,11 @@
         <v>0</v>
       </c>
       <c r="M41" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>(1, 1, 0, 1, 0, 0, 2, 0, 0, 0)</v>
       </c>
       <c r="O41">
-        <f>COUNTIF($M$2:$M$147,M41)</f>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
     </row>
@@ -3348,11 +3360,11 @@
         <v>0</v>
       </c>
       <c r="M42" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>(1, 1, 0, 1, 0, 0, 0, 0, 2, 0)</v>
       </c>
       <c r="O42">
-        <f>COUNTIF($M$2:$M$147,M42)</f>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
     </row>
@@ -3394,11 +3406,11 @@
         <v>0</v>
       </c>
       <c r="M43" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>(1, 1, 0, 1, 0, 0, 2, 0, 2, 0)</v>
       </c>
       <c r="O43">
-        <f>COUNTIF($M$2:$M$147,M43)</f>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
     </row>
@@ -3444,7 +3456,7 @@
         <v>(0, 0, 1, 0, 0, 0, 0, 0, 0, 0)</v>
       </c>
       <c r="O44">
-        <f>COUNTIF($M$2:$M$147,M44)</f>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
     </row>
@@ -3490,7 +3502,7 @@
         <v>(0, 0, 1, 0, 0, 0, 0, 0, 1, 0)</v>
       </c>
       <c r="O45">
-        <f>COUNTIF($M$2:$M$147,M45)</f>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
     </row>
@@ -3536,7 +3548,7 @@
         <v>(0, 0, 1, 0, 0, 0, 0, 0, 2, 0)</v>
       </c>
       <c r="O46">
-        <f>COUNTIF($M$2:$M$147,M46)</f>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
     </row>
@@ -3578,14 +3590,14 @@
         <v>0</v>
       </c>
       <c r="M47" t="str">
-        <f t="shared" ref="M47:M49" si="6">"("&amp;C47&amp;", "&amp;D47&amp;", "&amp;E47&amp;", "&amp;F47&amp;", "&amp;G47&amp;", "&amp;H47&amp;", "&amp;I47&amp;", "&amp;J47&amp;", "&amp;K47&amp;", "&amp;L47&amp;")"</f>
+        <f t="shared" ref="M47:M49" si="8">"("&amp;C47&amp;", "&amp;D47&amp;", "&amp;E47&amp;", "&amp;F47&amp;", "&amp;G47&amp;", "&amp;H47&amp;", "&amp;I47&amp;", "&amp;J47&amp;", "&amp;K47&amp;", "&amp;L47&amp;")"</f>
         <v>(1, 0, 1, 0, 0, 0, 0, 0, 0, 0)</v>
       </c>
       <c r="N47" t="s">
         <v>101</v>
       </c>
       <c r="O47">
-        <f>COUNTIF($M$2:$M$147,M47)</f>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
     </row>
@@ -3627,14 +3639,14 @@
         <v>0</v>
       </c>
       <c r="M48" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>(1, 0, 1, 0, 0, 0, 0, 0, 1, 0)</v>
       </c>
       <c r="N48" t="s">
         <v>101</v>
       </c>
       <c r="O48">
-        <f>COUNTIF($M$2:$M$147,M48)</f>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
     </row>
@@ -3676,14 +3688,14 @@
         <v>0</v>
       </c>
       <c r="M49" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>(1, 0, 1, 0, 0, 0, 0, 0, 2, 0)</v>
       </c>
       <c r="N49" t="s">
         <v>101</v>
       </c>
       <c r="O49">
-        <f>COUNTIF($M$2:$M$147,M49)</f>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
     </row>
@@ -3729,7 +3741,7 @@
         <v>(0, 0, 1, 0, 0, 0, 1, 0, 0, 0)</v>
       </c>
       <c r="O50">
-        <f>COUNTIF($M$2:$M$147,M50)</f>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
     </row>
@@ -3775,7 +3787,7 @@
         <v>(0, 0, 1, 0, 0, 0, 1, 0, 1, 0)</v>
       </c>
       <c r="O51">
-        <f>COUNTIF($M$2:$M$147,M51)</f>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
     </row>
@@ -3821,7 +3833,7 @@
         <v>(0, 0, 1, 0, 0, 0, 1, 0, 2, 0)</v>
       </c>
       <c r="O52">
-        <f>COUNTIF($M$2:$M$147,M52)</f>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
     </row>
@@ -3867,7 +3879,7 @@
         <v>(0, 0, 1, 0, 0, 0, 2, 0, 0, 0)</v>
       </c>
       <c r="O53">
-        <f>COUNTIF($M$2:$M$147,M53)</f>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
     </row>
@@ -3913,7 +3925,7 @@
         <v>(0, 0, 1, 0, 0, 0, 2, 0, 1, 0)</v>
       </c>
       <c r="O54">
-        <f>COUNTIF($M$2:$M$147,M54)</f>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
     </row>
@@ -3959,7 +3971,7 @@
         <v>(0, 0, 1, 0, 0, 0, 2, 0, 2, 0)</v>
       </c>
       <c r="O55">
-        <f>COUNTIF($M$2:$M$147,M55)</f>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
     </row>
@@ -4001,14 +4013,14 @@
         <v>0</v>
       </c>
       <c r="M56" t="str">
-        <f t="shared" ref="M56:M58" si="7">"("&amp;C56&amp;", "&amp;D56&amp;", "&amp;E56&amp;", "&amp;F56&amp;", "&amp;G56&amp;", "&amp;H56&amp;", "&amp;I56&amp;", "&amp;J56&amp;", "&amp;K56&amp;", "&amp;L56&amp;")"</f>
+        <f t="shared" ref="M56:M58" si="9">"("&amp;C56&amp;", "&amp;D56&amp;", "&amp;E56&amp;", "&amp;F56&amp;", "&amp;G56&amp;", "&amp;H56&amp;", "&amp;I56&amp;", "&amp;J56&amp;", "&amp;K56&amp;", "&amp;L56&amp;")"</f>
         <v>(1, 0, 1, 0, 0, 0, 2, 0, 0, 0)</v>
       </c>
       <c r="N56" t="s">
         <v>101</v>
       </c>
       <c r="O56">
-        <f>COUNTIF($M$2:$M$147,M56)</f>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
     </row>
@@ -4050,14 +4062,14 @@
         <v>0</v>
       </c>
       <c r="M57" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>(1, 0, 1, 0, 0, 0, 2, 0, 1, 0)</v>
       </c>
       <c r="N57" t="s">
         <v>101</v>
       </c>
       <c r="O57">
-        <f>COUNTIF($M$2:$M$147,M57)</f>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
     </row>
@@ -4099,14 +4111,14 @@
         <v>0</v>
       </c>
       <c r="M58" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>(1, 0, 1, 0, 0, 0, 2, 0, 2, 0)</v>
       </c>
       <c r="N58" t="s">
         <v>101</v>
       </c>
       <c r="O58">
-        <f>COUNTIF($M$2:$M$147,M58)</f>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
     </row>
@@ -4152,7 +4164,7 @@
         <v>(0, 1, 0, 0, 0, 0, 0, 0, 0, 0)</v>
       </c>
       <c r="O59">
-        <f>COUNTIF($M$2:$M$147,M59)</f>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
     </row>
@@ -4198,7 +4210,7 @@
         <v>(0, 1, 0, 0, 0, 0, 0, 0, 1, 0)</v>
       </c>
       <c r="O60">
-        <f>COUNTIF($M$2:$M$147,M60)</f>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
     </row>
@@ -4240,11 +4252,11 @@
         <v>0</v>
       </c>
       <c r="M61" t="str">
-        <f t="shared" ref="M61:M100" si="8">"("&amp;C61&amp;", "&amp;D61&amp;", "&amp;E61&amp;", "&amp;F61&amp;", "&amp;G61&amp;", "&amp;H61&amp;", "&amp;I61&amp;", "&amp;J61&amp;", "&amp;K61&amp;", "&amp;L61&amp;")"</f>
+        <f t="shared" ref="M61:M100" si="10">"("&amp;C61&amp;", "&amp;D61&amp;", "&amp;E61&amp;", "&amp;F61&amp;", "&amp;G61&amp;", "&amp;H61&amp;", "&amp;I61&amp;", "&amp;J61&amp;", "&amp;K61&amp;", "&amp;L61&amp;")"</f>
         <v>(0, 1, 0, 0, 0, 0, 0, 0, 2, 0)</v>
       </c>
       <c r="O61">
-        <f>COUNTIF($M$2:$M$147,M61)</f>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
     </row>
@@ -4286,11 +4298,11 @@
         <v>0</v>
       </c>
       <c r="M62" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>(1, 1, 0, 0, 0, 0, 0, 0, 0, 0)</v>
       </c>
       <c r="O62">
-        <f>COUNTIF($M$2:$M$147,M62)</f>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
     </row>
@@ -4332,11 +4344,11 @@
         <v>0</v>
       </c>
       <c r="M63" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>(1, 1, 0, 0, 0, 0, 0, 0, 1, 0)</v>
       </c>
       <c r="O63">
-        <f>COUNTIF($M$2:$M$147,M63)</f>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
     </row>
@@ -4378,11 +4390,11 @@
         <v>0</v>
       </c>
       <c r="M64" t="str">
-        <f t="shared" ref="M64" si="9">"("&amp;C64&amp;", "&amp;D64&amp;", "&amp;E64&amp;", "&amp;F64&amp;", "&amp;G64&amp;", "&amp;H64&amp;", "&amp;I64&amp;", "&amp;J64&amp;", "&amp;K64&amp;", "&amp;L64&amp;")"</f>
+        <f t="shared" ref="M64" si="11">"("&amp;C64&amp;", "&amp;D64&amp;", "&amp;E64&amp;", "&amp;F64&amp;", "&amp;G64&amp;", "&amp;H64&amp;", "&amp;I64&amp;", "&amp;J64&amp;", "&amp;K64&amp;", "&amp;L64&amp;")"</f>
         <v>(1, 1, 0, 0, 0, 0, 0, 0, 2, 0)</v>
       </c>
       <c r="O64">
-        <f>COUNTIF($M$2:$M$147,M64)</f>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
     </row>
@@ -4424,11 +4436,11 @@
         <v>0</v>
       </c>
       <c r="M65" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>(0, 1, 0, 0, 0, 0, 1, 0, 0, 0)</v>
       </c>
       <c r="O65">
-        <f>COUNTIF($M$2:$M$147,M65)</f>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
     </row>
@@ -4470,11 +4482,11 @@
         <v>0</v>
       </c>
       <c r="M66" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>(0, 1, 0, 0, 0, 0, 1, 0, 1, 0)</v>
       </c>
       <c r="O66">
-        <f>COUNTIF($M$2:$M$147,M66)</f>
+        <f t="shared" ref="O66:O97" si="12">COUNTIF($M$2:$M$147,M66)</f>
         <v>1</v>
       </c>
     </row>
@@ -4516,11 +4528,11 @@
         <v>0</v>
       </c>
       <c r="M67" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>(0, 1, 0, 0, 0, 0, 1, 0, 2, 0)</v>
       </c>
       <c r="O67">
-        <f>COUNTIF($M$2:$M$147,M67)</f>
+        <f t="shared" si="12"/>
         <v>1</v>
       </c>
     </row>
@@ -4562,11 +4574,11 @@
         <v>0</v>
       </c>
       <c r="M68" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>(0, 1, 0, 0, 0, 0, 2, 0, 0, 0)</v>
       </c>
       <c r="O68">
-        <f>COUNTIF($M$2:$M$147,M68)</f>
+        <f t="shared" si="12"/>
         <v>1</v>
       </c>
     </row>
@@ -4608,11 +4620,11 @@
         <v>0</v>
       </c>
       <c r="M69" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>(0, 1, 0, 0, 0, 0, 2, 0, 1, 0)</v>
       </c>
       <c r="O69">
-        <f>COUNTIF($M$2:$M$147,M69)</f>
+        <f t="shared" si="12"/>
         <v>1</v>
       </c>
     </row>
@@ -4654,11 +4666,11 @@
         <v>0</v>
       </c>
       <c r="M70" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>(0, 1, 0, 0, 0, 0, 2, 0, 2, 0)</v>
       </c>
       <c r="O70">
-        <f>COUNTIF($M$2:$M$147,M70)</f>
+        <f t="shared" si="12"/>
         <v>1</v>
       </c>
     </row>
@@ -4700,11 +4712,11 @@
         <v>0</v>
       </c>
       <c r="M71" t="str">
-        <f t="shared" ref="M71:M73" si="10">"("&amp;C71&amp;", "&amp;D71&amp;", "&amp;E71&amp;", "&amp;F71&amp;", "&amp;G71&amp;", "&amp;H71&amp;", "&amp;I71&amp;", "&amp;J71&amp;", "&amp;K71&amp;", "&amp;L71&amp;")"</f>
+        <f t="shared" ref="M71:M73" si="13">"("&amp;C71&amp;", "&amp;D71&amp;", "&amp;E71&amp;", "&amp;F71&amp;", "&amp;G71&amp;", "&amp;H71&amp;", "&amp;I71&amp;", "&amp;J71&amp;", "&amp;K71&amp;", "&amp;L71&amp;")"</f>
         <v>(1, 1, 0, 0, 0, 0, 2, 0, 0, 0)</v>
       </c>
       <c r="O71">
-        <f>COUNTIF($M$2:$M$147,M71)</f>
+        <f t="shared" si="12"/>
         <v>1</v>
       </c>
     </row>
@@ -4746,11 +4758,11 @@
         <v>0</v>
       </c>
       <c r="M72" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="13"/>
         <v>(1, 1, 0, 0, 0, 0, 2, 0, 1, 0)</v>
       </c>
       <c r="O72">
-        <f>COUNTIF($M$2:$M$147,M72)</f>
+        <f t="shared" si="12"/>
         <v>1</v>
       </c>
     </row>
@@ -4792,11 +4804,11 @@
         <v>0</v>
       </c>
       <c r="M73" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="13"/>
         <v>(1, 1, 0, 0, 0, 0, 2, 0, 2, 0)</v>
       </c>
       <c r="O73">
-        <f>COUNTIF($M$2:$M$147,M73)</f>
+        <f t="shared" si="12"/>
         <v>1</v>
       </c>
     </row>
@@ -4838,11 +4850,11 @@
         <v>0</v>
       </c>
       <c r="M74" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>(1, 0, 0, 0, 0, 0, 2, 0, 0, 0)</v>
       </c>
       <c r="O74">
-        <f>COUNTIF($M$2:$M$147,M74)</f>
+        <f t="shared" si="12"/>
         <v>1</v>
       </c>
     </row>
@@ -4884,11 +4896,11 @@
         <v>0</v>
       </c>
       <c r="M75" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>(1, 0, 0, 0, 0, 0, 2, 0, 1, 0)</v>
       </c>
       <c r="O75">
-        <f>COUNTIF($M$2:$M$147,M75)</f>
+        <f t="shared" si="12"/>
         <v>1</v>
       </c>
     </row>
@@ -4930,11 +4942,11 @@
         <v>0</v>
       </c>
       <c r="M76" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>(1, 0, 0, 0, 0, 0, 2, 0, 2, 0)</v>
       </c>
       <c r="O76">
-        <f>COUNTIF($M$2:$M$147,M76)</f>
+        <f t="shared" si="12"/>
         <v>1</v>
       </c>
     </row>
@@ -4976,11 +4988,11 @@
         <v>0</v>
       </c>
       <c r="M77" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>(1, 0, 0, 0, 0, 0, 0, 0, 0, 0)</v>
       </c>
       <c r="O77">
-        <f>COUNTIF($M$2:$M$147,M77)</f>
+        <f t="shared" si="12"/>
         <v>1</v>
       </c>
     </row>
@@ -5022,11 +5034,11 @@
         <v>0</v>
       </c>
       <c r="M78" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>(1, 0, 0, 0, 0, 0, 0, 0, 1, 0)</v>
       </c>
       <c r="O78">
-        <f>COUNTIF($M$2:$M$147,M78)</f>
+        <f t="shared" si="12"/>
         <v>1</v>
       </c>
     </row>
@@ -5068,11 +5080,11 @@
         <v>0</v>
       </c>
       <c r="M79" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>(1, 0, 0, 0, 0, 0, 0, 0, 2, 0)</v>
       </c>
       <c r="O79">
-        <f>COUNTIF($M$2:$M$147,M79)</f>
+        <f t="shared" si="12"/>
         <v>1</v>
       </c>
     </row>
@@ -5114,11 +5126,11 @@
         <v>0</v>
       </c>
       <c r="M80" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>(0, 1, 1, 0, 0, 0, 0, 0, 0, 0)</v>
       </c>
       <c r="O80">
-        <f>COUNTIF($M$2:$M$147,M80)</f>
+        <f t="shared" si="12"/>
         <v>1</v>
       </c>
     </row>
@@ -5160,11 +5172,11 @@
         <v>0</v>
       </c>
       <c r="M81" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>(0, 1, 1, 0, 0, 0, 0, 0, 1, 0)</v>
       </c>
       <c r="O81">
-        <f>COUNTIF($M$2:$M$147,M81)</f>
+        <f t="shared" si="12"/>
         <v>1</v>
       </c>
     </row>
@@ -5206,11 +5218,11 @@
         <v>0</v>
       </c>
       <c r="M82" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>(0, 1, 1, 0, 0, 0, 0, 0, 2, 0)</v>
       </c>
       <c r="O82">
-        <f>COUNTIF($M$2:$M$147,M82)</f>
+        <f t="shared" si="12"/>
         <v>1</v>
       </c>
     </row>
@@ -5252,11 +5264,11 @@
         <v>0</v>
       </c>
       <c r="M83" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>(0, 1, 1, 0, 0, 0, 1, 0, 0, 0)</v>
       </c>
       <c r="O83">
-        <f>COUNTIF($M$2:$M$147,M83)</f>
+        <f t="shared" si="12"/>
         <v>1</v>
       </c>
     </row>
@@ -5298,11 +5310,11 @@
         <v>0</v>
       </c>
       <c r="M84" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>(0, 1, 1, 0, 0, 0, 1, 0, 1, 0)</v>
       </c>
       <c r="O84">
-        <f>COUNTIF($M$2:$M$147,M84)</f>
+        <f t="shared" si="12"/>
         <v>1</v>
       </c>
     </row>
@@ -5344,11 +5356,11 @@
         <v>0</v>
       </c>
       <c r="M85" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>(0, 1, 1, 0, 0, 0, 1, 0, 2, 0)</v>
       </c>
       <c r="O85">
-        <f>COUNTIF($M$2:$M$147,M85)</f>
+        <f t="shared" si="12"/>
         <v>1</v>
       </c>
     </row>
@@ -5390,11 +5402,11 @@
         <v>0</v>
       </c>
       <c r="M86" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>(0, 1, 1, 0, 0, 0, 2, 0, 0, 0)</v>
       </c>
       <c r="O86">
-        <f>COUNTIF($M$2:$M$147,M86)</f>
+        <f t="shared" si="12"/>
         <v>1</v>
       </c>
     </row>
@@ -5436,11 +5448,11 @@
         <v>0</v>
       </c>
       <c r="M87" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>(0, 1, 1, 0, 0, 0, 2, 0, 1, 0)</v>
       </c>
       <c r="O87">
-        <f>COUNTIF($M$2:$M$147,M87)</f>
+        <f t="shared" si="12"/>
         <v>1</v>
       </c>
     </row>
@@ -5482,11 +5494,11 @@
         <v>0</v>
       </c>
       <c r="M88" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>(0, 1, 1, 0, 0, 0, 2, 0, 2, 0)</v>
       </c>
       <c r="O88">
-        <f>COUNTIF($M$2:$M$147,M88)</f>
+        <f t="shared" si="12"/>
         <v>1</v>
       </c>
     </row>
@@ -5528,11 +5540,11 @@
         <v>0</v>
       </c>
       <c r="M89" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>(0, 0, 0, 1, 0, 0, 0, 0, 0, 0)</v>
       </c>
       <c r="O89">
-        <f>COUNTIF($M$2:$M$147,M89)</f>
+        <f t="shared" si="12"/>
         <v>1</v>
       </c>
     </row>
@@ -5574,11 +5586,11 @@
         <v>0</v>
       </c>
       <c r="M90" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>(0, 0, 0, 1, 0, 0, 1, 0, 0, 0)</v>
       </c>
       <c r="O90">
-        <f>COUNTIF($M$2:$M$147,M90)</f>
+        <f t="shared" si="12"/>
         <v>1</v>
       </c>
     </row>
@@ -5620,11 +5632,11 @@
         <v>0</v>
       </c>
       <c r="M91" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>(0, 0, 0, 1, 0, 0, 2, 0, 0, 0)</v>
       </c>
       <c r="O91">
-        <f>COUNTIF($M$2:$M$147,M91)</f>
+        <f t="shared" si="12"/>
         <v>1</v>
       </c>
     </row>
@@ -5666,11 +5678,11 @@
         <v>0</v>
       </c>
       <c r="M92" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>(0, 0, 0, 1, 0, 0, 0, 0, 2, 0)</v>
       </c>
       <c r="O92">
-        <f>COUNTIF($M$2:$M$147,M92)</f>
+        <f t="shared" si="12"/>
         <v>1</v>
       </c>
     </row>
@@ -5712,11 +5724,11 @@
         <v>0</v>
       </c>
       <c r="M93" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>(0, 0, 0, 1, 0, 0, 1, 0, 2, 0)</v>
       </c>
       <c r="O93">
-        <f>COUNTIF($M$2:$M$147,M93)</f>
+        <f t="shared" si="12"/>
         <v>1</v>
       </c>
     </row>
@@ -5758,11 +5770,11 @@
         <v>0</v>
       </c>
       <c r="M94" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>(0, 0, 0, 1, 0, 0, 2, 0, 2, 0)</v>
       </c>
       <c r="O94">
-        <f>COUNTIF($M$2:$M$147,M94)</f>
+        <f t="shared" si="12"/>
         <v>1</v>
       </c>
     </row>
@@ -5804,11 +5816,11 @@
         <v>0</v>
       </c>
       <c r="M95" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>(0, 0, 0, 1, 0, 0, 0, 0, 1, 0)</v>
       </c>
       <c r="O95">
-        <f>COUNTIF($M$2:$M$147,M95)</f>
+        <f t="shared" si="12"/>
         <v>1</v>
       </c>
     </row>
@@ -5850,11 +5862,11 @@
         <v>0</v>
       </c>
       <c r="M96" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>(0, 0, 0, 1, 0, 0, 1, 0, 1, 0)</v>
       </c>
       <c r="O96">
-        <f>COUNTIF($M$2:$M$147,M96)</f>
+        <f t="shared" si="12"/>
         <v>1</v>
       </c>
     </row>
@@ -5896,11 +5908,11 @@
         <v>0</v>
       </c>
       <c r="M97" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>(0, 0, 0, 1, 0, 0, 2, 0, 1, 0)</v>
       </c>
       <c r="O97">
-        <f>COUNTIF($M$2:$M$147,M97)</f>
+        <f t="shared" si="12"/>
         <v>1</v>
       </c>
     </row>
@@ -5942,14 +5954,14 @@
         <v>0</v>
       </c>
       <c r="M98" t="str">
-        <f t="shared" ref="M98:M99" si="11">"("&amp;C98&amp;", "&amp;D98&amp;", "&amp;E98&amp;", "&amp;F98&amp;", "&amp;G98&amp;", "&amp;H98&amp;", "&amp;I98&amp;", "&amp;J98&amp;", "&amp;K98&amp;", "&amp;L98&amp;")"</f>
+        <f t="shared" ref="M98:M99" si="14">"("&amp;C98&amp;", "&amp;D98&amp;", "&amp;E98&amp;", "&amp;F98&amp;", "&amp;G98&amp;", "&amp;H98&amp;", "&amp;I98&amp;", "&amp;J98&amp;", "&amp;K98&amp;", "&amp;L98&amp;")"</f>
         <v>(1, 0, 0, 1, 0, 0, 0, 0, 1, 0)</v>
       </c>
       <c r="N98" t="s">
         <v>101</v>
       </c>
       <c r="O98">
-        <f>COUNTIF($M$2:$M$147,M98)</f>
+        <f t="shared" ref="O98:O129" si="15">COUNTIF($M$2:$M$147,M98)</f>
         <v>1</v>
       </c>
     </row>
@@ -5991,14 +6003,14 @@
         <v>0</v>
       </c>
       <c r="M99" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="14"/>
         <v>(1, 0, 0, 1, 0, 0, 2, 0, 1, 0)</v>
       </c>
       <c r="N99" t="s">
         <v>101</v>
       </c>
       <c r="O99">
-        <f>COUNTIF($M$2:$M$147,M99)</f>
+        <f t="shared" si="15"/>
         <v>1</v>
       </c>
     </row>
@@ -6040,11 +6052,11 @@
         <v>0</v>
       </c>
       <c r="M100" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>(1, 0, 0, 0, 0, 0, 1, 0, 0, 0)</v>
       </c>
       <c r="O100">
-        <f>COUNTIF($M$2:$M$147,M100)</f>
+        <f t="shared" si="15"/>
         <v>1</v>
       </c>
     </row>
@@ -6086,11 +6098,11 @@
         <v>0</v>
       </c>
       <c r="M101" t="str">
-        <f t="shared" ref="M101:M130" si="12">"("&amp;C101&amp;", "&amp;D101&amp;", "&amp;E101&amp;", "&amp;F101&amp;", "&amp;G101&amp;", "&amp;H101&amp;", "&amp;I101&amp;", "&amp;J101&amp;", "&amp;K101&amp;", "&amp;L101&amp;")"</f>
+        <f t="shared" ref="M101:M130" si="16">"("&amp;C101&amp;", "&amp;D101&amp;", "&amp;E101&amp;", "&amp;F101&amp;", "&amp;G101&amp;", "&amp;H101&amp;", "&amp;I101&amp;", "&amp;J101&amp;", "&amp;K101&amp;", "&amp;L101&amp;")"</f>
         <v>(1, 0, 0, 0, 0, 0, 1, 0, 1, 0)</v>
       </c>
       <c r="O101">
-        <f>COUNTIF($M$2:$M$147,M101)</f>
+        <f t="shared" si="15"/>
         <v>1</v>
       </c>
     </row>
@@ -6132,11 +6144,11 @@
         <v>0</v>
       </c>
       <c r="M102" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="16"/>
         <v>(1, 0, 0, 0, 0, 0, 1, 0, 2, 0)</v>
       </c>
       <c r="O102">
-        <f>COUNTIF($M$2:$M$147,M102)</f>
+        <f t="shared" si="15"/>
         <v>1</v>
       </c>
     </row>
@@ -6178,11 +6190,11 @@
         <v>0</v>
       </c>
       <c r="M103" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="16"/>
         <v>(1, 0, 0, 1, 1, 1, 1, 0, 0, 0)</v>
       </c>
       <c r="O103">
-        <f>COUNTIF($M$2:$M$147,M103)</f>
+        <f t="shared" si="15"/>
         <v>1</v>
       </c>
     </row>
@@ -6224,11 +6236,11 @@
         <v>0</v>
       </c>
       <c r="M104" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="16"/>
         <v>(1, 0, 0, 1, 1, 0, 1, 0, 0, 0)</v>
       </c>
       <c r="O104">
-        <f>COUNTIF($M$2:$M$147,M104)</f>
+        <f t="shared" si="15"/>
         <v>1</v>
       </c>
     </row>
@@ -6270,11 +6282,11 @@
         <v>0</v>
       </c>
       <c r="M105" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="16"/>
         <v>(1, 0, 0, 1, 1, 1, 1, 0, 2, 0)</v>
       </c>
       <c r="O105">
-        <f>COUNTIF($M$2:$M$147,M105)</f>
+        <f t="shared" si="15"/>
         <v>1</v>
       </c>
     </row>
@@ -6316,11 +6328,11 @@
         <v>0</v>
       </c>
       <c r="M106" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="16"/>
         <v>(1, 0, 0, 1, 1, 0, 1, 0, 2, 0)</v>
       </c>
       <c r="O106">
-        <f>COUNTIF($M$2:$M$147,M106)</f>
+        <f t="shared" si="15"/>
         <v>1</v>
       </c>
     </row>
@@ -6362,11 +6374,11 @@
         <v>0</v>
       </c>
       <c r="M107" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="16"/>
         <v>(1, 0, 0, 1, 0, 0, 1, 0, 0, 0)</v>
       </c>
       <c r="O107">
-        <f>COUNTIF($M$2:$M$147,M107)</f>
+        <f t="shared" si="15"/>
         <v>1</v>
       </c>
     </row>
@@ -6408,14 +6420,14 @@
         <v>0</v>
       </c>
       <c r="M108" t="str">
-        <f t="shared" ref="M108" si="13">"("&amp;C108&amp;", "&amp;D108&amp;", "&amp;E108&amp;", "&amp;F108&amp;", "&amp;G108&amp;", "&amp;H108&amp;", "&amp;I108&amp;", "&amp;J108&amp;", "&amp;K108&amp;", "&amp;L108&amp;")"</f>
+        <f t="shared" ref="M108" si="17">"("&amp;C108&amp;", "&amp;D108&amp;", "&amp;E108&amp;", "&amp;F108&amp;", "&amp;G108&amp;", "&amp;H108&amp;", "&amp;I108&amp;", "&amp;J108&amp;", "&amp;K108&amp;", "&amp;L108&amp;")"</f>
         <v>(1, 0, 0, 1, 0, 0, 1, 0, 2, 0)</v>
       </c>
       <c r="N108" t="s">
         <v>101</v>
       </c>
       <c r="O108">
-        <f>COUNTIF($M$2:$M$147,M108)</f>
+        <f t="shared" si="15"/>
         <v>1</v>
       </c>
     </row>
@@ -6457,11 +6469,11 @@
         <v>0</v>
       </c>
       <c r="M109" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="16"/>
         <v>(1, 1, 1, 0, 0, 0, 1, 0, 0, 0)</v>
       </c>
       <c r="O109">
-        <f>COUNTIF($M$2:$M$147,M109)</f>
+        <f t="shared" si="15"/>
         <v>1</v>
       </c>
     </row>
@@ -6503,11 +6515,11 @@
         <v>0</v>
       </c>
       <c r="M110" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="16"/>
         <v>(1, 1, 1, 0, 0, 0, 1, 0, 1, 0)</v>
       </c>
       <c r="O110">
-        <f>COUNTIF($M$2:$M$147,M110)</f>
+        <f t="shared" si="15"/>
         <v>1</v>
       </c>
     </row>
@@ -6549,11 +6561,11 @@
         <v>0</v>
       </c>
       <c r="M111" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="16"/>
         <v>(1, 1, 1, 0, 0, 0, 1, 0, 2, 0)</v>
       </c>
       <c r="O111">
-        <f>COUNTIF($M$2:$M$147,M111)</f>
+        <f t="shared" si="15"/>
         <v>1</v>
       </c>
     </row>
@@ -6595,11 +6607,11 @@
         <v>0</v>
       </c>
       <c r="M112" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="16"/>
         <v>(1, 0, 1, 0, 0, 0, 1, 0, 0, 0)</v>
       </c>
       <c r="O112">
-        <f>COUNTIF($M$2:$M$147,M112)</f>
+        <f t="shared" si="15"/>
         <v>1</v>
       </c>
     </row>
@@ -6641,11 +6653,11 @@
         <v>0</v>
       </c>
       <c r="M113" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="16"/>
         <v>(1, 0, 1, 0, 0, 0, 1, 0, 1, 0)</v>
       </c>
       <c r="O113">
-        <f>COUNTIF($M$2:$M$147,M113)</f>
+        <f t="shared" si="15"/>
         <v>1</v>
       </c>
     </row>
@@ -6687,11 +6699,11 @@
         <v>0</v>
       </c>
       <c r="M114" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="16"/>
         <v>(1, 0, 1, 0, 0, 0, 1, 0, 2, 0)</v>
       </c>
       <c r="O114">
-        <f>COUNTIF($M$2:$M$147,M114)</f>
+        <f t="shared" si="15"/>
         <v>1</v>
       </c>
     </row>
@@ -6733,11 +6745,11 @@
         <v>0</v>
       </c>
       <c r="M115" t="str">
-        <f t="shared" ref="M115:M117" si="14">"("&amp;C115&amp;", "&amp;D115&amp;", "&amp;E115&amp;", "&amp;F115&amp;", "&amp;G115&amp;", "&amp;H115&amp;", "&amp;I115&amp;", "&amp;J115&amp;", "&amp;K115&amp;", "&amp;L115&amp;")"</f>
+        <f t="shared" ref="M115:M117" si="18">"("&amp;C115&amp;", "&amp;D115&amp;", "&amp;E115&amp;", "&amp;F115&amp;", "&amp;G115&amp;", "&amp;H115&amp;", "&amp;I115&amp;", "&amp;J115&amp;", "&amp;K115&amp;", "&amp;L115&amp;")"</f>
         <v>(1, 1, 0, 0, 0, 0, 1, 0, 0, 0)</v>
       </c>
       <c r="O115">
-        <f>COUNTIF($M$2:$M$147,M115)</f>
+        <f t="shared" si="15"/>
         <v>1</v>
       </c>
     </row>
@@ -6779,11 +6791,11 @@
         <v>0</v>
       </c>
       <c r="M116" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="18"/>
         <v>(1, 1, 0, 0, 0, 0, 1, 0, 1, 0)</v>
       </c>
       <c r="O116">
-        <f>COUNTIF($M$2:$M$147,M116)</f>
+        <f t="shared" si="15"/>
         <v>1</v>
       </c>
     </row>
@@ -6825,11 +6837,11 @@
         <v>0</v>
       </c>
       <c r="M117" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="18"/>
         <v>(1, 1, 0, 0, 0, 0, 1, 0, 2, 0)</v>
       </c>
       <c r="O117">
-        <f>COUNTIF($M$2:$M$147,M117)</f>
+        <f t="shared" si="15"/>
         <v>1</v>
       </c>
     </row>
@@ -6871,11 +6883,11 @@
         <v>0</v>
       </c>
       <c r="M118" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="16"/>
         <v>(1, 0, 0, 0, 0, 0, 0, 99, 0, 0)</v>
       </c>
       <c r="O118">
-        <f>COUNTIF($M$2:$M$147,M118)</f>
+        <f t="shared" si="15"/>
         <v>1</v>
       </c>
     </row>
@@ -6917,11 +6929,11 @@
         <v>0</v>
       </c>
       <c r="M119" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="16"/>
         <v>(1, 0, 0, 0, 0, 0, 0, 99, 1, 0)</v>
       </c>
       <c r="O119">
-        <f>COUNTIF($M$2:$M$147,M119)</f>
+        <f t="shared" si="15"/>
         <v>1</v>
       </c>
     </row>
@@ -6963,11 +6975,11 @@
         <v>0</v>
       </c>
       <c r="M120" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="16"/>
         <v>(1, 0, 0, 0, 0, 0, 0, 99, 2, 0)</v>
       </c>
       <c r="O120">
-        <f>COUNTIF($M$2:$M$147,M120)</f>
+        <f t="shared" si="15"/>
         <v>1</v>
       </c>
     </row>
@@ -7009,11 +7021,11 @@
         <v>0</v>
       </c>
       <c r="M121" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="16"/>
         <v>(1, 1, 1, 0, 0, 0, 2, 0, 0, 0)</v>
       </c>
       <c r="O121">
-        <f>COUNTIF($M$2:$M$147,M121)</f>
+        <f t="shared" si="15"/>
         <v>1</v>
       </c>
     </row>
@@ -7055,11 +7067,11 @@
         <v>0</v>
       </c>
       <c r="M122" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="16"/>
         <v>(1, 1, 1, 0, 0, 0, 2, 0, 1, 0)</v>
       </c>
       <c r="O122">
-        <f>COUNTIF($M$2:$M$147,M122)</f>
+        <f t="shared" si="15"/>
         <v>1</v>
       </c>
     </row>
@@ -7101,11 +7113,11 @@
         <v>0</v>
       </c>
       <c r="M123" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="16"/>
         <v>(1, 1, 1, 0, 0, 0, 2, 0, 2, 0)</v>
       </c>
       <c r="O123">
-        <f>COUNTIF($M$2:$M$147,M123)</f>
+        <f t="shared" si="15"/>
         <v>1</v>
       </c>
     </row>
@@ -7147,11 +7159,11 @@
         <v>0</v>
       </c>
       <c r="M124" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="16"/>
         <v>(1, 1, 1, 0, 0, 0, 0, 0, 0, 0)</v>
       </c>
       <c r="O124">
-        <f>COUNTIF($M$2:$M$147,M124)</f>
+        <f t="shared" si="15"/>
         <v>1</v>
       </c>
     </row>
@@ -7193,11 +7205,11 @@
         <v>0</v>
       </c>
       <c r="M125" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="16"/>
         <v>(1, 1, 1, 0, 0, 0, 0, 0, 1, 0)</v>
       </c>
       <c r="O125">
-        <f>COUNTIF($M$2:$M$147,M125)</f>
+        <f t="shared" si="15"/>
         <v>1</v>
       </c>
     </row>
@@ -7239,11 +7251,11 @@
         <v>0</v>
       </c>
       <c r="M126" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="16"/>
         <v>(1, 1, 1, 0, 0, 0, 0, 0, 2, 0)</v>
       </c>
       <c r="O126">
-        <f>COUNTIF($M$2:$M$147,M126)</f>
+        <f t="shared" si="15"/>
         <v>1</v>
       </c>
     </row>
@@ -7285,11 +7297,11 @@
         <v>0</v>
       </c>
       <c r="M127" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="16"/>
         <v>(0, 0, 0, 0, 0, 0, 0, 0, 0, 0)</v>
       </c>
       <c r="O127">
-        <f>COUNTIF($M$2:$M$147,M127)</f>
+        <f t="shared" si="15"/>
         <v>1</v>
       </c>
     </row>
@@ -7331,11 +7343,11 @@
         <v>0</v>
       </c>
       <c r="M128" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="16"/>
         <v>(0, 0, 0, 0, 0, 0, 2, 0, 0, 0)</v>
       </c>
       <c r="O128">
-        <f>COUNTIF($M$2:$M$147,M128)</f>
+        <f t="shared" si="15"/>
         <v>1</v>
       </c>
     </row>
@@ -7377,11 +7389,11 @@
         <v>0</v>
       </c>
       <c r="M129" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="16"/>
         <v>(0, 0, 0, 0, 0, 0, 1, 0, 0, 0)</v>
       </c>
       <c r="O129">
-        <f>COUNTIF($M$2:$M$147,M129)</f>
+        <f t="shared" si="15"/>
         <v>1</v>
       </c>
     </row>
@@ -7423,11 +7435,11 @@
         <v>0</v>
       </c>
       <c r="M130" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="16"/>
         <v>(0, 0, 0, 0, 0, 0, 0, 0, 2, 0)</v>
       </c>
       <c r="O130">
-        <f>COUNTIF($M$2:$M$147,M130)</f>
+        <f t="shared" ref="O130:O147" si="19">COUNTIF($M$2:$M$147,M130)</f>
         <v>1</v>
       </c>
     </row>
@@ -7469,11 +7481,11 @@
         <v>0</v>
       </c>
       <c r="M131" t="str">
-        <f t="shared" ref="M131:M132" si="15">"("&amp;C131&amp;", "&amp;D131&amp;", "&amp;E131&amp;", "&amp;F131&amp;", "&amp;G131&amp;", "&amp;H131&amp;", "&amp;I131&amp;", "&amp;J131&amp;", "&amp;K131&amp;", "&amp;L131&amp;")"</f>
+        <f t="shared" ref="M131:M132" si="20">"("&amp;C131&amp;", "&amp;D131&amp;", "&amp;E131&amp;", "&amp;F131&amp;", "&amp;G131&amp;", "&amp;H131&amp;", "&amp;I131&amp;", "&amp;J131&amp;", "&amp;K131&amp;", "&amp;L131&amp;")"</f>
         <v>(0, 0, 0, 0, 0, 0, 2, 0, 2, 0)</v>
       </c>
       <c r="O131">
-        <f>COUNTIF($M$2:$M$147,M131)</f>
+        <f t="shared" si="19"/>
         <v>1</v>
       </c>
     </row>
@@ -7515,11 +7527,11 @@
         <v>0</v>
       </c>
       <c r="M132" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="20"/>
         <v>(0, 0, 0, 0, 0, 0, 1, 0, 2, 0)</v>
       </c>
       <c r="O132">
-        <f>COUNTIF($M$2:$M$147,M132)</f>
+        <f t="shared" si="19"/>
         <v>1</v>
       </c>
     </row>
@@ -7561,11 +7573,11 @@
         <v>0</v>
       </c>
       <c r="M133" t="str">
-        <f t="shared" ref="M133:M141" si="16">"("&amp;C133&amp;", "&amp;D133&amp;", "&amp;E133&amp;", "&amp;F133&amp;", "&amp;G133&amp;", "&amp;H133&amp;", "&amp;I133&amp;", "&amp;J133&amp;", "&amp;K133&amp;", "&amp;L133&amp;")"</f>
+        <f t="shared" ref="M133:M141" si="21">"("&amp;C133&amp;", "&amp;D133&amp;", "&amp;E133&amp;", "&amp;F133&amp;", "&amp;G133&amp;", "&amp;H133&amp;", "&amp;I133&amp;", "&amp;J133&amp;", "&amp;K133&amp;", "&amp;L133&amp;")"</f>
         <v>(0, 0, 0, 0, 0, 0, 0, 0, 1, 0)</v>
       </c>
       <c r="O133">
-        <f>COUNTIF($M$2:$M$147,M133)</f>
+        <f t="shared" si="19"/>
         <v>1</v>
       </c>
     </row>
@@ -7607,11 +7619,11 @@
         <v>0</v>
       </c>
       <c r="M134" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="21"/>
         <v>(0, 0, 0, 0, 0, 0, 2, 0, 1, 0)</v>
       </c>
       <c r="O134">
-        <f>COUNTIF($M$2:$M$147,M134)</f>
+        <f t="shared" si="19"/>
         <v>1</v>
       </c>
     </row>
@@ -7653,11 +7665,11 @@
         <v>0</v>
       </c>
       <c r="M135" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="21"/>
         <v>(0, 0, 0, 0, 0, 0, 1, 0, 1, 0)</v>
       </c>
       <c r="O135">
-        <f>COUNTIF($M$2:$M$147,M135)</f>
+        <f t="shared" si="19"/>
         <v>1</v>
       </c>
     </row>
@@ -7699,14 +7711,14 @@
         <v>0</v>
       </c>
       <c r="M136" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="21"/>
         <v>(0, 0, 0, 0, 1, 0, 0, 0, 0, 0)</v>
       </c>
       <c r="N136" t="s">
         <v>101</v>
       </c>
       <c r="O136">
-        <f>COUNTIF($M$2:$M$147,M136)</f>
+        <f t="shared" si="19"/>
         <v>1</v>
       </c>
     </row>
@@ -7748,14 +7760,14 @@
         <v>0</v>
       </c>
       <c r="M137" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="21"/>
         <v>(0, 0, 0, 0, 1, 0, 2, 0, 0, 0)</v>
       </c>
       <c r="N137" t="s">
         <v>101</v>
       </c>
       <c r="O137">
-        <f>COUNTIF($M$2:$M$147,M137)</f>
+        <f t="shared" si="19"/>
         <v>1</v>
       </c>
     </row>
@@ -7797,14 +7809,14 @@
         <v>0</v>
       </c>
       <c r="M138" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="21"/>
         <v>(0, 0, 0, 0, 1, 1, 0, 0, 0, 0)</v>
       </c>
       <c r="N138" t="s">
         <v>101</v>
       </c>
       <c r="O138">
-        <f>COUNTIF($M$2:$M$147,M138)</f>
+        <f t="shared" si="19"/>
         <v>1</v>
       </c>
     </row>
@@ -7846,14 +7858,14 @@
         <v>0</v>
       </c>
       <c r="M139" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="21"/>
         <v>(0, 0, 0, 0, 1, 1, 2, 0, 0, 0)</v>
       </c>
       <c r="N139" t="s">
         <v>101</v>
       </c>
       <c r="O139">
-        <f>COUNTIF($M$2:$M$147,M139)</f>
+        <f t="shared" si="19"/>
         <v>1</v>
       </c>
     </row>
@@ -7895,14 +7907,14 @@
         <v>0</v>
       </c>
       <c r="M140" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="21"/>
         <v>(1, 0, 0, 0, 1, 0, 2, 0, 0, 0)</v>
       </c>
       <c r="N140" t="s">
         <v>101</v>
       </c>
       <c r="O140">
-        <f>COUNTIF($M$2:$M$147,M140)</f>
+        <f t="shared" si="19"/>
         <v>1</v>
       </c>
     </row>
@@ -7944,14 +7956,14 @@
         <v>0</v>
       </c>
       <c r="M141" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="21"/>
         <v>(1, 0, 0, 0, 1, 0, 0, 0, 0, 0)</v>
       </c>
       <c r="N141" t="s">
         <v>101</v>
       </c>
       <c r="O141">
-        <f>COUNTIF($M$2:$M$147,M141)</f>
+        <f t="shared" si="19"/>
         <v>1</v>
       </c>
     </row>
@@ -8000,7 +8012,7 @@
         <v>101</v>
       </c>
       <c r="O142">
-        <f>COUNTIF($M$2:$M$147,M142)</f>
+        <f t="shared" si="19"/>
         <v>1</v>
       </c>
     </row>
@@ -8042,14 +8054,14 @@
         <v>0</v>
       </c>
       <c r="M143" t="str">
-        <f t="shared" ref="M143:M147" si="17">"("&amp;C143&amp;", "&amp;D143&amp;", "&amp;E143&amp;", "&amp;F143&amp;", "&amp;G143&amp;", "&amp;H143&amp;", "&amp;I143&amp;", "&amp;J143&amp;", "&amp;K143&amp;", "&amp;L143&amp;")"</f>
+        <f t="shared" ref="M143:M147" si="22">"("&amp;C143&amp;", "&amp;D143&amp;", "&amp;E143&amp;", "&amp;F143&amp;", "&amp;G143&amp;", "&amp;H143&amp;", "&amp;I143&amp;", "&amp;J143&amp;", "&amp;K143&amp;", "&amp;L143&amp;")"</f>
         <v>(1, 0, 0, 0, 1, 1, 0, 0, 0, 0)</v>
       </c>
       <c r="N143" t="s">
         <v>101</v>
       </c>
       <c r="O143">
-        <f>COUNTIF($M$2:$M$147,M143)</f>
+        <f t="shared" si="19"/>
         <v>1</v>
       </c>
     </row>
@@ -8091,14 +8103,14 @@
         <v>0</v>
       </c>
       <c r="M144" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="22"/>
         <v>(1, 1, 1, 1, 0, 0, 1, 0, 0, 0)</v>
       </c>
       <c r="N144" t="s">
         <v>101</v>
       </c>
       <c r="O144">
-        <f>COUNTIF($M$2:$M$147,M144)</f>
+        <f t="shared" si="19"/>
         <v>1</v>
       </c>
     </row>
@@ -8140,14 +8152,14 @@
         <v>0</v>
       </c>
       <c r="M145" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="22"/>
         <v>(0, 1, 1, 1, 0, 0, 1, 0, 0, 0)</v>
       </c>
       <c r="N145" t="s">
         <v>101</v>
       </c>
       <c r="O145">
-        <f>COUNTIF($M$2:$M$147,M145)</f>
+        <f t="shared" si="19"/>
         <v>1</v>
       </c>
     </row>
@@ -8189,14 +8201,14 @@
         <v>0</v>
       </c>
       <c r="M146" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="22"/>
         <v>(1, 1, 1, 1, 0, 0, 1, 0, 2, 0)</v>
       </c>
       <c r="N146" t="s">
         <v>101</v>
       </c>
       <c r="O146">
-        <f>COUNTIF($M$2:$M$147,M146)</f>
+        <f t="shared" si="19"/>
         <v>1</v>
       </c>
     </row>
@@ -8238,14 +8250,210 @@
         <v>0</v>
       </c>
       <c r="M147" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="22"/>
         <v>(0, 1, 1, 1, 0, 0, 1, 0, 2, 0)</v>
       </c>
       <c r="N147" t="s">
         <v>101</v>
       </c>
       <c r="O147">
-        <f>COUNTIF($M$2:$M$147,M147)</f>
+        <f t="shared" si="19"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="148" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A148" t="s">
+        <v>161</v>
+      </c>
+      <c r="B148">
+        <v>35</v>
+      </c>
+      <c r="C148">
+        <v>1</v>
+      </c>
+      <c r="D148">
+        <v>1</v>
+      </c>
+      <c r="E148">
+        <v>0</v>
+      </c>
+      <c r="F148">
+        <v>1</v>
+      </c>
+      <c r="G148">
+        <v>0</v>
+      </c>
+      <c r="H148">
+        <v>0</v>
+      </c>
+      <c r="I148">
+        <v>1</v>
+      </c>
+      <c r="J148">
+        <v>0</v>
+      </c>
+      <c r="K148">
+        <v>0</v>
+      </c>
+      <c r="L148">
+        <v>0</v>
+      </c>
+      <c r="M148" t="str">
+        <f t="shared" ref="M148:M163" si="23">"("&amp;C148&amp;", "&amp;D148&amp;", "&amp;E148&amp;", "&amp;F148&amp;", "&amp;G148&amp;", "&amp;H148&amp;", "&amp;I148&amp;", "&amp;J148&amp;", "&amp;K148&amp;", "&amp;L148&amp;")"</f>
+        <v>(1, 1, 0, 1, 0, 0, 1, 0, 0, 0)</v>
+      </c>
+      <c r="N148" t="s">
+        <v>101</v>
+      </c>
+      <c r="O148">
+        <f>COUNTIF($M$2:$M$163,M148)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="149" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A149" t="s">
+        <v>162</v>
+      </c>
+      <c r="B149">
+        <v>26</v>
+      </c>
+      <c r="C149">
+        <v>1</v>
+      </c>
+      <c r="D149">
+        <v>0</v>
+      </c>
+      <c r="E149">
+        <v>1</v>
+      </c>
+      <c r="F149">
+        <v>1</v>
+      </c>
+      <c r="G149">
+        <v>0</v>
+      </c>
+      <c r="H149">
+        <v>0</v>
+      </c>
+      <c r="I149">
+        <v>1</v>
+      </c>
+      <c r="J149">
+        <v>0</v>
+      </c>
+      <c r="K149">
+        <v>0</v>
+      </c>
+      <c r="L149">
+        <v>0</v>
+      </c>
+      <c r="M149" t="str">
+        <f t="shared" si="23"/>
+        <v>(1, 0, 1, 1, 0, 0, 1, 0, 0, 0)</v>
+      </c>
+      <c r="N149" t="s">
+        <v>101</v>
+      </c>
+      <c r="O149">
+        <f>COUNTIF($M$2:$M$163,M149)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="150" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A150" t="s">
+        <v>163</v>
+      </c>
+      <c r="B150">
+        <v>35</v>
+      </c>
+      <c r="C150">
+        <v>1</v>
+      </c>
+      <c r="D150">
+        <v>1</v>
+      </c>
+      <c r="E150">
+        <v>0</v>
+      </c>
+      <c r="F150">
+        <v>1</v>
+      </c>
+      <c r="G150">
+        <v>0</v>
+      </c>
+      <c r="H150">
+        <v>0</v>
+      </c>
+      <c r="I150">
+        <v>1</v>
+      </c>
+      <c r="J150">
+        <v>0</v>
+      </c>
+      <c r="K150">
+        <v>2</v>
+      </c>
+      <c r="L150">
+        <v>0</v>
+      </c>
+      <c r="M150" t="str">
+        <f t="shared" ref="M150:M151" si="24">"("&amp;C150&amp;", "&amp;D150&amp;", "&amp;E150&amp;", "&amp;F150&amp;", "&amp;G150&amp;", "&amp;H150&amp;", "&amp;I150&amp;", "&amp;J150&amp;", "&amp;K150&amp;", "&amp;L150&amp;")"</f>
+        <v>(1, 1, 0, 1, 0, 0, 1, 0, 2, 0)</v>
+      </c>
+      <c r="N150" t="s">
+        <v>101</v>
+      </c>
+      <c r="O150">
+        <f>COUNTIF($M$2:$M$163,M150)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="151" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A151" t="s">
+        <v>164</v>
+      </c>
+      <c r="B151">
+        <v>26</v>
+      </c>
+      <c r="C151">
+        <v>1</v>
+      </c>
+      <c r="D151">
+        <v>0</v>
+      </c>
+      <c r="E151">
+        <v>1</v>
+      </c>
+      <c r="F151">
+        <v>1</v>
+      </c>
+      <c r="G151">
+        <v>0</v>
+      </c>
+      <c r="H151">
+        <v>0</v>
+      </c>
+      <c r="I151">
+        <v>1</v>
+      </c>
+      <c r="J151">
+        <v>0</v>
+      </c>
+      <c r="K151">
+        <v>2</v>
+      </c>
+      <c r="L151">
+        <v>0</v>
+      </c>
+      <c r="M151" t="str">
+        <f t="shared" si="24"/>
+        <v>(1, 0, 1, 1, 0, 0, 1, 0, 2, 0)</v>
+      </c>
+      <c r="N151" t="s">
+        <v>101</v>
+      </c>
+      <c r="O151">
+        <f>COUNTIF($M$2:$M$163,M151)</f>
         <v>1</v>
       </c>
     </row>

</xml_diff>